<commit_message>
rerunning analysis and creating figures using the final flume dataset.
</commit_message>
<xml_diff>
--- a/data/scratch/hoeRain.xlsx
+++ b/data/scratch/hoeRain.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="hoeRain" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F137" sqref="F137"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D457" sqref="D419:D457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>